<commit_message>
adaugare program Andrei Marica
</commit_message>
<xml_diff>
--- a/Program+Traineri_Z2H_2017.xlsx
+++ b/Program+Traineri_Z2H_2017.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>Know your language - OOP</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>Radu Hoaghe</t>
+  </si>
+  <si>
+    <t>Andrei Marica (?)</t>
+  </si>
+  <si>
+    <t>Andrei Marica</t>
   </si>
 </sst>
 </file>
@@ -509,17 +515,17 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="29.25" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="68.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="62.5703125" customWidth="1"/>
-    <col min="5" max="5" width="44.140625" customWidth="1"/>
+    <col min="2" max="2" width="68.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="62.5546875" customWidth="1"/>
+    <col min="5" max="5" width="44.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -536,7 +542,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -544,7 +550,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -552,7 +558,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -565,7 +571,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -578,7 +584,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -591,7 +597,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -604,18 +610,20 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -625,10 +633,12 @@
       <c r="C9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -638,10 +648,12 @@
       <c r="C10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -652,7 +664,7 @@
       <c r="D11" s="2"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -663,7 +675,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -674,7 +686,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -685,7 +697,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -696,7 +708,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -707,7 +719,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -715,10 +727,12 @@
         <v>8</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -726,10 +740,12 @@
         <v>9</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="D18" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -737,10 +753,12 @@
         <v>10</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -748,10 +766,12 @@
         <v>11</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -774,7 +794,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -786,7 +806,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adaugata sesiunea de git
</commit_message>
<xml_diff>
--- a/Program+Traineri_Z2H_2017.xlsx
+++ b/Program+Traineri_Z2H_2017.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>Know your language - OOP</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>Radu Hoaghe, Cristian Dumitru(?)</t>
+  </si>
+  <si>
+    <t>Git</t>
   </si>
 </sst>
 </file>
@@ -533,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="29.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -563,41 +566,39 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1">
-        <v>1</v>
+    <row r="2" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="5" t="s">
@@ -607,10 +608,10 @@
     </row>
     <row r="6" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="5" t="s">
@@ -620,10 +621,10 @@
     </row>
     <row r="7" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="5" t="s">
@@ -633,116 +634,118 @@
     </row>
     <row r="8" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>35</v>
+        <v>21</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E9" s="1"/>
     </row>
     <row r="10" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="1"/>
     </row>
     <row r="13" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -750,23 +753,21 @@
     </row>
     <row r="17" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="D17" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="D17" s="2"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
@@ -776,40 +777,53 @@
     </row>
     <row r="19" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="1"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update - adaugat coloana cu data estimativa pentru fiecare sesiune.
</commit_message>
<xml_diff>
--- a/Program+Traineri_Z2H_2017.xlsx
+++ b/Program+Traineri_Z2H_2017.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="521"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
   <si>
     <t>Know your language - OOP</t>
   </si>
@@ -167,6 +167,72 @@
   </si>
   <si>
     <t>Gentiana Mecu</t>
+  </si>
+  <si>
+    <t>2017.06.26</t>
+  </si>
+  <si>
+    <t>2017.06.27</t>
+  </si>
+  <si>
+    <t>2017.06.28</t>
+  </si>
+  <si>
+    <t>2017.06.29</t>
+  </si>
+  <si>
+    <t>2017.06.30</t>
+  </si>
+  <si>
+    <t>2017.07.03</t>
+  </si>
+  <si>
+    <t>2017.07.04</t>
+  </si>
+  <si>
+    <t>2017.07.05</t>
+  </si>
+  <si>
+    <t>2017.07.06</t>
+  </si>
+  <si>
+    <t>2017.07.07</t>
+  </si>
+  <si>
+    <t>2017.07.10</t>
+  </si>
+  <si>
+    <t>2017.07.11</t>
+  </si>
+  <si>
+    <t>2017.07.12</t>
+  </si>
+  <si>
+    <t>2017.07.13</t>
+  </si>
+  <si>
+    <t>2017.07.14</t>
+  </si>
+  <si>
+    <t>2017.07.17</t>
+  </si>
+  <si>
+    <t>2017.07.18</t>
+  </si>
+  <si>
+    <t>2017.07.19</t>
+  </si>
+  <si>
+    <t>2017.07.20</t>
+  </si>
+  <si>
+    <t>2017.07.21</t>
+  </si>
+  <si>
+    <t>2017.07.24</t>
+  </si>
+  <si>
+    <t>Data estimativa</t>
   </si>
 </sst>
 </file>
@@ -560,320 +626,387 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="29.25" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="68.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="62.5703125" customWidth="1"/>
-    <col min="5" max="5" width="44.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="62.5546875" customWidth="1"/>
+    <col min="6" max="6" width="44.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+    <row r="4" spans="1:6" s="1" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="1"/>
+      <c r="E7" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12">
         <v>10</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13">
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14">
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16">
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17">
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="E17" s="2"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18">
         <v>16</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19">
         <v>17</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20">
         <v>18</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21">
         <v>19</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="2"/>
+      <c r="E21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22">
         <v>20</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="1"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -887,7 +1020,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -899,7 +1032,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixat curs de sql
</commit_message>
<xml_diff>
--- a/Program+Traineri_Z2H_2017.xlsx
+++ b/Program+Traineri_Z2H_2017.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="354"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="354"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -200,12 +200,6 @@
   </si>
   <si>
     <t>Tacliciu Viorel</t>
-  </si>
-  <si>
-    <t>Radu Sezciuc</t>
-  </si>
-  <si>
-    <t>Oana Besliu, Mihai Tudose, Mihai Vaduva</t>
   </si>
   <si>
     <t>Radu Hoaghe, Cristian Dumitru(?), Bianca Ambrosa, Daniel Ioan Ivan, Mihai Tudose, Hanna Botar</t>
@@ -282,6 +276,12 @@
   </si>
   <si>
     <t>Cristian Dumitru(?), Bianca Ambrosa, Daniel Ioan Ivan, Mihai Tudose, Hanna Botar</t>
+  </si>
+  <si>
+    <t>Anca Neamtu</t>
+  </si>
+  <si>
+    <t>Madalin Purice, Carmen Bonciog, Nicoleta Fusea</t>
   </si>
 </sst>
 </file>
@@ -319,14 +319,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,11 +344,6 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -369,11 +365,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -384,14 +379,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -696,19 +686,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="29.25" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="62.5703125" customWidth="1"/>
-    <col min="6" max="6" width="44.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="62.5546875" customWidth="1"/>
+    <col min="6" max="6" width="44.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -728,7 +718,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -742,11 +732,11 @@
         <v>55</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" s="1" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -760,10 +750,10 @@
         <v>31</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -777,11 +767,11 @@
         <v>29</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -795,11 +785,11 @@
         <v>29</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -810,14 +800,14 @@
         <v>20</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -828,14 +818,14 @@
         <v>21</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -846,14 +836,14 @@
         <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -867,11 +857,11 @@
         <v>26</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -882,14 +872,14 @@
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -903,11 +893,11 @@
         <v>27</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -921,29 +911,28 @@
         <v>30</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -957,11 +946,11 @@
         <v>54</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>45</v>
       </c>
@@ -975,11 +964,11 @@
         <v>29</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>46</v>
       </c>
@@ -993,11 +982,11 @@
         <v>29</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F16" s="1"/>
     </row>
-    <row r="17" spans="1:6" s="1" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="1" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>47</v>
       </c>
@@ -1011,10 +1000,10 @@
         <v>55</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -1028,11 +1017,11 @@
         <v>28</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>49</v>
       </c>
@@ -1046,11 +1035,11 @@
         <v>28</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -1064,11 +1053,11 @@
         <v>56</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -1082,11 +1071,11 @@
         <v>56</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -1100,7 +1089,7 @@
         <v>56</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F22" s="1"/>
     </row>
@@ -1116,7 +1105,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1128,7 +1117,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>